<commit_message>
Basic logic is working Added another recipe in the test data
</commit_message>
<xml_diff>
--- a/recipes.xlsx
+++ b/recipes.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/majkenandersen/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krose\Repositories\opskrifter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D779C0AE-DB49-E24B-A68E-C182110A3782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB2E316-32F7-4958-9FF4-D127CB5A0B26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{1DF9BAFE-AC5C-E845-B4CA-1FB82D7DF7D2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{1DF9BAFE-AC5C-E845-B4CA-1FB82D7DF7D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Retter" sheetId="1" r:id="rId1"/>
     <sheet name="Ingredienser" sheetId="2" r:id="rId2"/>
     <sheet name="Forbrug" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="40">
   <si>
     <t>ID</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Navn</t>
   </si>
   <si>
-    <t>Måleenhed</t>
-  </si>
-  <si>
     <t>RetID</t>
   </si>
   <si>
@@ -132,6 +129,33 @@
   </si>
   <si>
     <t>Panko</t>
+  </si>
+  <si>
+    <t>Enhed</t>
+  </si>
+  <si>
+    <t>Jasminris</t>
+  </si>
+  <si>
+    <t>Spinat</t>
+  </si>
+  <si>
+    <t>pose(r)</t>
+  </si>
+  <si>
+    <t>Gulerod</t>
+  </si>
+  <si>
+    <t>Forårsløg</t>
+  </si>
+  <si>
+    <t>Sesamfrø</t>
+  </si>
+  <si>
+    <t>Sojasauce</t>
+  </si>
+  <si>
+    <t>Mayonaise</t>
   </si>
 </sst>
 </file>
@@ -187,7 +211,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -489,13 +513,13 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -503,17 +527,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -526,15 +550,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA1D6F3A-C42A-9249-9195-C7F544F55CEE}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -542,191 +566,271 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>8</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>9</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>11</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>12</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12">
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13">
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14">
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15">
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16">
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17">
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B18">
         <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -736,278 +840,689 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46356CDD-C11E-954C-B72D-1CB56AB59220}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>24</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>25</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <f>VLOOKUP(Forbrug!B2,Retter!A:B,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
         <f>VLOOKUP(D2,Ingredienser!A:C,2,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" t="str">
+        <f>VLOOKUP(D2,Ingredienser!A:C,3,FALSE)</f>
+        <v>stk</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <f>VLOOKUP(Forbrug!B3,Retter!A:B,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3">
+        <v>1000</v>
+      </c>
+      <c r="F3">
         <f>VLOOKUP(D3,Ingredienser!A:C,2,FALSE)</f>
         <v>2</v>
       </c>
-      <c r="F3">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" t="str">
+        <f>VLOOKUP(D3,Ingredienser!A:C,3,FALSE)</f>
+        <v>gram</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <f>VLOOKUP(Forbrug!B4,Retter!A:B,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
         <f>VLOOKUP(D4,Ingredienser!A:C,2,FALSE)</f>
         <v>3</v>
       </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" t="str">
+        <f>VLOOKUP(D4,Ingredienser!A:C,3,FALSE)</f>
+        <v>stk</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5">
         <f>VLOOKUP(Forbrug!B5,Retter!A:B,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
         <f>VLOOKUP(D5,Ingredienser!A:C,2,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" t="str">
+        <f>VLOOKUP(D5,Ingredienser!A:C,3,FALSE)</f>
+        <v>fed</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <f>VLOOKUP(Forbrug!B6,Retter!A:B,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
         <f>VLOOKUP(D6,Ingredienser!A:C,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" t="str">
+        <f>VLOOKUP(D6,Ingredienser!A:C,3,FALSE)</f>
+        <v>stk</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7">
         <f>VLOOKUP(Forbrug!B7,Retter!A:B,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E7">
+        <v>250</v>
+      </c>
+      <c r="F7">
         <f>VLOOKUP(D7,Ingredienser!A:C,2,FALSE)</f>
         <v>6</v>
       </c>
-      <c r="F7">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" t="str">
+        <f>VLOOKUP(D7,Ingredienser!A:C,3,FALSE)</f>
+        <v>dl</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8">
         <f>VLOOKUP(Forbrug!B8,Retter!A:B,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E8">
+        <v>500</v>
+      </c>
+      <c r="F8">
         <f>VLOOKUP(D8,Ingredienser!A:C,2,FALSE)</f>
         <v>7</v>
       </c>
-      <c r="F8">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" t="str">
+        <f>VLOOKUP(D8,Ingredienser!A:C,3,FALSE)</f>
+        <v>gram</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9">
         <f>VLOOKUP(Forbrug!B9,Retter!A:B,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
         <f>VLOOKUP(D9,Ingredienser!A:C,2,FALSE)</f>
         <v>8</v>
       </c>
-      <c r="F9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9" t="str">
+        <f>VLOOKUP(D9,Ingredienser!A:C,3,FALSE)</f>
+        <v>gram</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10">
         <f>VLOOKUP(Forbrug!B10,Retter!A:B,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10">
         <f>VLOOKUP(D10,Ingredienser!A:C,2,FALSE)</f>
         <v>9</v>
       </c>
-      <c r="F10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10" t="str">
+        <f>VLOOKUP(D10,Ingredienser!A:C,3,FALSE)</f>
+        <v>stk</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11">
         <f>VLOOKUP(Forbrug!B11,Retter!A:B,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
         <f>VLOOKUP(D11,Ingredienser!A:C,2,FALSE)</f>
         <v>10</v>
       </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" t="str">
+        <f>VLOOKUP(D11,Ingredienser!A:C,3,FALSE)</f>
+        <v>pose</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12">
         <f>VLOOKUP(Forbrug!B12,Retter!A:B,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E12">
+        <v>25</v>
+      </c>
+      <c r="F12">
         <f>VLOOKUP(D12,Ingredienser!A:C,2,FALSE)</f>
         <v>11</v>
       </c>
-      <c r="F12">
-        <v>25</v>
+      <c r="G12" t="str">
+        <f>VLOOKUP(D12,Ingredienser!A:C,3,FALSE)</f>
+        <v>ml</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13">
+        <f>VLOOKUP(Forbrug!B13,Retter!A:B,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13">
+        <v>5</v>
+      </c>
+      <c r="F13">
+        <f>VLOOKUP(D13,Ingredienser!A:C,2,FALSE)</f>
+        <v>12</v>
+      </c>
+      <c r="G13" t="str">
+        <f>VLOOKUP(D13,Ingredienser!A:C,3,FALSE)</f>
+        <v>gram</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14">
+        <f>VLOOKUP(Forbrug!B14,Retter!A:B,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14">
+        <v>80</v>
+      </c>
+      <c r="F14">
+        <f>VLOOKUP(D14,Ingredienser!A:C,2,FALSE)</f>
+        <v>13</v>
+      </c>
+      <c r="G14" t="str">
+        <f>VLOOKUP(D14,Ingredienser!A:C,3,FALSE)</f>
+        <v>gram</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15">
+        <f>VLOOKUP(Forbrug!B15,Retter!A:B,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15">
+        <v>50</v>
+      </c>
+      <c r="F15">
+        <f>VLOOKUP(D15,Ingredienser!A:C,2,FALSE)</f>
+        <v>14</v>
+      </c>
+      <c r="G15" t="str">
+        <f>VLOOKUP(D15,Ingredienser!A:C,3,FALSE)</f>
+        <v>gram</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16">
+        <f>VLOOKUP(Forbrug!B16,Retter!A:B,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <f>VLOOKUP(D16,Ingredienser!A:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="G16" t="str">
+        <f>VLOOKUP(D16,Ingredienser!A:C,3,FALSE)</f>
+        <v>stk</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17">
+        <f>VLOOKUP(Forbrug!B17,Retter!A:B,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17">
+        <v>100</v>
+      </c>
+      <c r="F17">
+        <f>VLOOKUP(D17,Ingredienser!A:C,2,FALSE)</f>
+        <v>16</v>
+      </c>
+      <c r="G17" t="str">
+        <f>VLOOKUP(D17,Ingredienser!A:C,3,FALSE)</f>
+        <v>gram</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18">
+        <f>VLOOKUP(Forbrug!B18,Retter!A:B,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18">
+        <v>4</v>
+      </c>
+      <c r="F18">
+        <f>VLOOKUP(D18,Ingredienser!A:C,2,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="G18" t="str">
+        <f>VLOOKUP(D18,Ingredienser!A:C,3,FALSE)</f>
+        <v>fed</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19">
+        <f>VLOOKUP(Forbrug!B19,Retter!A:B,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19">
+        <v>300</v>
+      </c>
+      <c r="F19">
+        <f>VLOOKUP(D19,Ingredienser!A:C,2,FALSE)</f>
+        <v>18</v>
+      </c>
+      <c r="G19" t="str">
+        <f>VLOOKUP(D19,Ingredienser!A:C,3,FALSE)</f>
+        <v>gram</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20">
+        <f>VLOOKUP(Forbrug!B20,Retter!A:B,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <f>VLOOKUP(D20,Ingredienser!A:C,2,FALSE)</f>
+        <v>19</v>
+      </c>
+      <c r="G20" t="str">
+        <f>VLOOKUP(D20,Ingredienser!A:C,3,FALSE)</f>
+        <v>pose(r)</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21">
+        <f>VLOOKUP(Forbrug!B21,Retter!A:B,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="F21">
+        <f>VLOOKUP(D21,Ingredienser!A:C,2,FALSE)</f>
+        <v>20</v>
+      </c>
+      <c r="G21" t="str">
+        <f>VLOOKUP(D21,Ingredienser!A:C,3,FALSE)</f>
+        <v>stk</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22">
+        <f>VLOOKUP(Forbrug!B22,Retter!A:B,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22">
+        <v>3</v>
+      </c>
+      <c r="F22">
+        <f>VLOOKUP(D22,Ingredienser!A:C,2,FALSE)</f>
+        <v>21</v>
+      </c>
+      <c r="G22" t="str">
+        <f>VLOOKUP(D22,Ingredienser!A:C,3,FALSE)</f>
+        <v>stk</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23">
+        <f>VLOOKUP(Forbrug!B23,Retter!A:B,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <f>VLOOKUP(D23,Ingredienser!A:C,2,FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="G23" t="str">
+        <f>VLOOKUP(D23,Ingredienser!A:C,3,FALSE)</f>
+        <v>stk</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24">
+        <f>VLOOKUP(Forbrug!B24,Retter!A:B,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24">
+        <v>20</v>
+      </c>
+      <c r="F24">
+        <f>VLOOKUP(D24,Ingredienser!A:C,2,FALSE)</f>
+        <v>22</v>
+      </c>
+      <c r="G24" t="str">
+        <f>VLOOKUP(D24,Ingredienser!A:C,3,FALSE)</f>
+        <v>gram</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25">
+        <f>VLOOKUP(Forbrug!B25,Retter!A:B,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="D25" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25">
+        <v>50</v>
+      </c>
+      <c r="F25">
+        <f>VLOOKUP(D25,Ingredienser!A:C,2,FALSE)</f>
+        <v>23</v>
+      </c>
+      <c r="G25" t="str">
+        <f>VLOOKUP(D25,Ingredienser!A:C,3,FALSE)</f>
+        <v>ml</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <f>VLOOKUP(Forbrug!B26,Retter!A:B,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26">
+        <v>50</v>
+      </c>
+      <c r="F26">
+        <f>VLOOKUP(D26,Ingredienser!A:C,2,FALSE)</f>
+        <v>24</v>
+      </c>
+      <c r="G26" t="str">
+        <f>VLOOKUP(D26,Ingredienser!A:C,3,FALSE)</f>
+        <v>gram</v>
       </c>
     </row>
   </sheetData>

</xml_diff>